<commit_message>
Support for google forms added
It works, just make sure your google form is setup correctly.
</commit_message>
<xml_diff>
--- a/R/PairwiseShinyApp/votes.xlsx
+++ b/R/PairwiseShinyApp/votes.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500" firstSheet="16" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sarah" sheetId="1" r:id="rId1"/>
-    <sheet name="Blaine" sheetId="2" r:id="rId2"/>
-    <sheet name="Christian" sheetId="3" r:id="rId3"/>
-    <sheet name="Alijah" sheetId="4" r:id="rId4"/>
-    <sheet name="Drew" sheetId="5" r:id="rId5"/>
+    <sheet name="Sarah1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blaine1" sheetId="2" r:id="rId2"/>
+    <sheet name="Christian1" sheetId="3" r:id="rId3"/>
+    <sheet name="Alijah1" sheetId="4" r:id="rId4"/>
+    <sheet name="Drew1" sheetId="5" r:id="rId5"/>
     <sheet name="Bradley" sheetId="6" r:id="rId6"/>
     <sheet name="Landon" sheetId="7" r:id="rId7"/>
     <sheet name="Liam" sheetId="8" r:id="rId8"/>
@@ -31,9 +31,8 @@
     <sheet name="Percy" sheetId="22" r:id="rId22"/>
     <sheet name="Sequoyah" sheetId="23" r:id="rId23"/>
     <sheet name="Aidan.H" sheetId="24" r:id="rId24"/>
-    <sheet name="info" sheetId="27" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="15">
   <si>
     <t>Math</t>
   </si>
@@ -88,87 +87,6 @@
   </si>
   <si>
     <t>pink</t>
-  </si>
-  <si>
-    <t>Bradley</t>
-  </si>
-  <si>
-    <t>Landon</t>
-  </si>
-  <si>
-    <t>Liam</t>
-  </si>
-  <si>
-    <t>Vaughn</t>
-  </si>
-  <si>
-    <t>Ceci</t>
-  </si>
-  <si>
-    <t>Madison</t>
-  </si>
-  <si>
-    <t>KayLynn</t>
-  </si>
-  <si>
-    <t>Maya</t>
-  </si>
-  <si>
-    <t>Gianna</t>
-  </si>
-  <si>
-    <t>Keira</t>
-  </si>
-  <si>
-    <t>Uriel</t>
-  </si>
-  <si>
-    <t>Olivia</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Elias</t>
-  </si>
-  <si>
-    <t>Drake</t>
-  </si>
-  <si>
-    <t>Angelique</t>
-  </si>
-  <si>
-    <t>Percy</t>
-  </si>
-  <si>
-    <t>Sequoyah</t>
-  </si>
-  <si>
-    <t>Aidan.H</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>Blaine</t>
-  </si>
-  <si>
-    <t>Christian</t>
-  </si>
-  <si>
-    <t>Alijah</t>
-  </si>
-  <si>
-    <t>Drew</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
 </sst>
 </file>
@@ -2282,7 +2200,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A8" sqref="A8:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2376,322 +2294,6 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="str">
-        <f>Sarah!$B$7</f>
-        <v>blue</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="str">
-        <f>Blaine!$B$7</f>
-        <v>green</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="str">
-        <f>Christian!B7</f>
-        <v>red</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="str">
-        <f>Alijah!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="str">
-        <f>Drew!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="str">
-        <f>Bradley!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="str">
-        <f>Landon!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="str">
-        <f>Liam!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="str">
-        <f>Vaughn!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="str">
-        <f>Ceci!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="str">
-        <f>Madison!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="str">
-        <f>KayLynn!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="str">
-        <f>Maya!B7</f>
-        <v>purple</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="str">
-        <f>Gianna!B7</f>
-        <v>purple</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="str">
-        <f>Keira!B7</f>
-        <v>blue</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="str">
-        <f>Uriel!B7</f>
-        <v>green</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="str">
-        <f>Olivia!B7</f>
-        <v>pink</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="str">
-        <f>James!B7</f>
-        <v>green</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="str">
-        <f>Elias!B7</f>
-        <v>green</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" t="str">
-        <f>Drake!B7</f>
-        <v>green</v>
-      </c>
-      <c r="C21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="str">
-        <f>Angelique!B7</f>
-        <v>pink</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" t="str">
-        <f>Percy!B7</f>
-        <v>green</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" t="str">
-        <f>Sequoyah!B7</f>
-        <v>purple</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="str">
-        <f>Aidan.H!B7</f>
-        <v>red</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2911,7 +2513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixing vote uploading bugs
Two problems, I stopped copying the new excel file, and instead loaded,
and second I reset the file upload, so you can upload the same file
again.
</commit_message>
<xml_diff>
--- a/R/PairwiseShinyApp/votes.xlsx
+++ b/R/PairwiseShinyApp/votes.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500" firstSheet="16" activeTab="24"/>
   </bookViews>
   <sheets>
-    <sheet name="Sarah1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blaine1" sheetId="2" r:id="rId2"/>
-    <sheet name="Christian1" sheetId="3" r:id="rId3"/>
-    <sheet name="Alijah1" sheetId="4" r:id="rId4"/>
-    <sheet name="Drew1" sheetId="5" r:id="rId5"/>
+    <sheet name="Sarah" sheetId="1" r:id="rId1"/>
+    <sheet name="Blaine" sheetId="2" r:id="rId2"/>
+    <sheet name="Christian" sheetId="3" r:id="rId3"/>
+    <sheet name="Alijah" sheetId="4" r:id="rId4"/>
+    <sheet name="Drew" sheetId="5" r:id="rId5"/>
     <sheet name="Bradley" sheetId="6" r:id="rId6"/>
     <sheet name="Landon" sheetId="7" r:id="rId7"/>
     <sheet name="Liam" sheetId="8" r:id="rId8"/>
@@ -31,8 +31,9 @@
     <sheet name="Percy" sheetId="22" r:id="rId22"/>
     <sheet name="Sequoyah" sheetId="23" r:id="rId23"/>
     <sheet name="Aidan.H" sheetId="24" r:id="rId24"/>
+    <sheet name="info" sheetId="27" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="42">
   <si>
     <t>Math</t>
   </si>
@@ -87,6 +88,87 @@
   </si>
   <si>
     <t>pink</t>
+  </si>
+  <si>
+    <t>Bradley</t>
+  </si>
+  <si>
+    <t>Landon</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>Vaughn</t>
+  </si>
+  <si>
+    <t>Ceci</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>KayLynn</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t>Gianna</t>
+  </si>
+  <si>
+    <t>Keira</t>
+  </si>
+  <si>
+    <t>Uriel</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Elias</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>Angelique</t>
+  </si>
+  <si>
+    <t>Percy</t>
+  </si>
+  <si>
+    <t>Sequoyah</t>
+  </si>
+  <si>
+    <t>Aidan.H</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Blaine</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Alijah</t>
+  </si>
+  <si>
+    <t>Drew</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -466,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -550,6 +632,12 @@
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2200,7 +2288,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2294,6 +2382,322 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="str">
+        <f>Sarah!$B$7</f>
+        <v>blue</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="str">
+        <f>Blaine!$B$7</f>
+        <v>green</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="str">
+        <f>Christian!B7</f>
+        <v>red</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="str">
+        <f>Alijah!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="str">
+        <f>Drew!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="str">
+        <f>Bradley!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="str">
+        <f>Landon!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="str">
+        <f>Liam!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="str">
+        <f>Vaughn!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="str">
+        <f>Ceci!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="str">
+        <f>Madison!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="str">
+        <f>KayLynn!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="str">
+        <f>Maya!B7</f>
+        <v>purple</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="str">
+        <f>Gianna!B7</f>
+        <v>purple</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="str">
+        <f>Keira!B7</f>
+        <v>blue</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="str">
+        <f>Uriel!B7</f>
+        <v>green</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="str">
+        <f>Olivia!B7</f>
+        <v>pink</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="str">
+        <f>James!B7</f>
+        <v>green</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="str">
+        <f>Elias!B7</f>
+        <v>green</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="str">
+        <f>Drake!B7</f>
+        <v>green</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="str">
+        <f>Angelique!B7</f>
+        <v>pink</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="str">
+        <f>Percy!B7</f>
+        <v>green</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="str">
+        <f>Sequoyah!B7</f>
+        <v>purple</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="str">
+        <f>Aidan.H!B7</f>
+        <v>red</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2513,7 +2917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>